<commit_message>
added dual package FET to replace diode and single FET to reduce part count.
</commit_message>
<xml_diff>
--- a/PCB/BoilermakeBadge_BOM.xlsx
+++ b/PCB/BoilermakeBadge_BOM.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Limao\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14232"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Digikey Parts List</t>
   </si>
@@ -54,12 +49,6 @@
   </si>
   <si>
     <t>Micro USB Type B</t>
-  </si>
-  <si>
-    <t>85-1001-6-ND</t>
-  </si>
-  <si>
-    <t>MOSFET P-ch, low R</t>
   </si>
   <si>
     <t>BC3AAAW-ND</t>
@@ -131,12 +120,6 @@
     </r>
   </si>
   <si>
-    <t>478-7805-1-ND</t>
-  </si>
-  <si>
-    <t>Diode (Sch), 1A, 1206</t>
-  </si>
-  <si>
     <t>296-14020-1-ND</t>
   </si>
   <si>
@@ -159,16 +142,22 @@
   </si>
   <si>
     <t>LED yellow, 1206</t>
+  </si>
+  <si>
+    <t>Dual MOSFET, P&amp;N, low Ron</t>
+  </si>
+  <si>
+    <t>FDS8958ADKR-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,7 +274,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -320,7 +309,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -497,32 +486,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -539,7 +528,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -557,7 +546,7 @@
         <v>3.96</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -571,34 +560,34 @@
         <v>1</v>
       </c>
       <c r="E4" s="3">
-        <f t="shared" ref="E4:E13" si="0">C4*D4</f>
+        <f t="shared" ref="E4:E11" si="0">C4*D4</f>
         <v>0.26</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="C5" s="2">
-        <v>0.12</v>
+        <v>0.41</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" s="3">
         <f t="shared" si="0"/>
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2">
         <v>1.0900000000000001</v>
@@ -611,12 +600,12 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C7" s="2">
         <v>0.19</v>
@@ -629,12 +618,12 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" s="2">
         <v>7.0000000000000007E-2</v>
@@ -647,12 +636,12 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C9" s="2">
         <v>0.09</v>
@@ -665,12 +654,12 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C10" s="2">
         <v>7.0000000000000007E-2</v>
@@ -683,12 +672,12 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C11" s="2">
         <v>7.0000000000000007E-2</v>
@@ -701,12 +690,12 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C12" s="2">
         <v>0.01</v>
@@ -719,12 +708,12 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C13" s="2">
         <v>0.02</v>
@@ -737,12 +726,12 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C14" s="2">
         <v>0.03</v>
@@ -755,50 +744,32 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C15" s="2">
-        <v>0.17</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" s="3">
         <f>C15*D15</f>
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="D16">
-        <v>2</v>
-      </c>
-      <c r="E16" s="3">
-        <f>C16*D16</f>
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="D26" s="1" t="s">
+    <row r="25" spans="1:5">
+      <c r="A25" s="1"/>
+      <c r="D25" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="3">
-        <f>SUM(E3:E25)</f>
-        <v>7.3800000000000017</v>
+      <c r="E25" s="3">
+        <f>SUM(E3:E24)</f>
+        <v>7.5000000000000018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added second PCB design.
</commit_message>
<xml_diff>
--- a/PCB/BoilermakeBadge_BOM.xlsx
+++ b/PCB/BoilermakeBadge_BOM.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Limao\Documents\GitHub\BoilerMakeBadge_I\PCB\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14232"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Digikey Parts List</t>
   </si>
@@ -120,12 +125,6 @@
     </r>
   </si>
   <si>
-    <t>296-14020-1-ND</t>
-  </si>
-  <si>
-    <t>74HC164 8-bit shiftregister</t>
-  </si>
-  <si>
     <t>160-1643-1-ND</t>
   </si>
   <si>
@@ -148,16 +147,28 @@
   </si>
   <si>
     <t>FDS8958ADKR-ND</t>
+  </si>
+  <si>
+    <t>568-3968-5-ND</t>
+  </si>
+  <si>
+    <t>74HC595 8-bit shiftregister</t>
+  </si>
+  <si>
+    <t>PCE3878DKR-ND</t>
+  </si>
+  <si>
+    <t>Al CAP 10uF 16v 20% SMD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,11 +219,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -486,32 +498,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.109375" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -528,7 +540,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -546,7 +558,7 @@
         <v>3.96</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -564,12 +576,12 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C5" s="2">
         <v>0.41</v>
@@ -582,7 +594,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -600,7 +612,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -618,7 +630,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -636,12 +648,12 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9" s="2">
         <v>0.09</v>
@@ -654,12 +666,12 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" s="2">
         <v>7.0000000000000007E-2</v>
@@ -672,12 +684,12 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C11" s="2">
         <v>7.0000000000000007E-2</v>
@@ -690,7 +702,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -708,7 +720,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -726,7 +738,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -744,32 +756,50 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C15" s="2">
-        <v>0.14000000000000001</v>
+        <v>0.1716</v>
       </c>
       <c r="D15">
         <v>2</v>
       </c>
       <c r="E15" s="3">
         <f>C15*D15</f>
-        <v>0.28000000000000003</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>0.34320000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.11527999999999999</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" s="3">
+        <f>C16*D16</f>
+        <v>0.23055999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="D25" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E25" s="3">
         <f>SUM(E3:E24)</f>
-        <v>7.5000000000000018</v>
+        <v>7.7937600000000016</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding square-ish layout variant with BM logo
</commit_message>
<xml_diff>
--- a/PCB/BoilermakeBadge_BOM.xlsx
+++ b/PCB/BoilermakeBadge_BOM.xlsx
@@ -163,9 +163,6 @@
     <t>10118193-0001LF</t>
   </si>
   <si>
-    <t>USBMicroB1</t>
-  </si>
-  <si>
     <t>FDS8958A</t>
   </si>
   <si>
@@ -178,9 +175,6 @@
     <t>BC3AAAW</t>
   </si>
   <si>
-    <t>Battery1</t>
-  </si>
-  <si>
     <t>HOLDER BATT 3AAA WIRE LEAD 6"</t>
   </si>
   <si>
@@ -437,6 +431,12 @@
   </si>
   <si>
     <t>BoilerMakeBoard_I</t>
+  </si>
+  <si>
+    <t>USB</t>
+  </si>
+  <si>
+    <t>Battery</t>
   </si>
 </sst>
 </file>
@@ -491,6 +491,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -862,7 +863,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,18 +882,18 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -974,7 +975,7 @@
         <v>41</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>42</v>
+        <v>132</v>
       </c>
       <c r="F6" t="s">
         <v>35</v>
@@ -983,13 +984,13 @@
         <v>2</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J6" s="11" t="s">
         <v>40</v>
       </c>
       <c r="K6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1000,10 +1001,10 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F7" t="s">
         <v>35</v>
@@ -1012,13 +1013,13 @@
         <v>10</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -1029,10 +1030,10 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>47</v>
+        <v>133</v>
       </c>
       <c r="F8" t="s">
         <v>35</v>
@@ -1041,13 +1042,13 @@
         <v>3</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1058,10 +1059,10 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F9" t="s">
         <v>35</v>
@@ -1070,13 +1071,13 @@
         <v>4</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -1087,10 +1088,10 @@
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F10" t="s">
         <v>35</v>
@@ -1102,10 +1103,10 @@
         <v>1206</v>
       </c>
       <c r="J10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1116,10 +1117,10 @@
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F11" t="s">
         <v>35</v>
@@ -1131,10 +1132,10 @@
         <v>1206</v>
       </c>
       <c r="J11" t="s">
+        <v>62</v>
+      </c>
+      <c r="K11" t="s">
         <v>64</v>
-      </c>
-      <c r="K11" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1145,10 +1146,10 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>71</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>73</v>
       </c>
       <c r="F12" t="s">
         <v>35</v>
@@ -1157,13 +1158,13 @@
         <v>7</v>
       </c>
       <c r="I12" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="K12" t="s">
         <v>67</v>
-      </c>
-      <c r="J12" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="K12" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1174,10 +1175,10 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F13" t="s">
         <v>35</v>
@@ -1192,7 +1193,7 @@
         <v>9</v>
       </c>
       <c r="K13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1203,25 +1204,25 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F14" t="s">
         <v>35</v>
       </c>
       <c r="G14" t="s">
+        <v>72</v>
+      </c>
+      <c r="I14" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="I14" s="13" t="s">
-        <v>76</v>
-      </c>
       <c r="J14" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="K14" t="s">
         <v>75</v>
-      </c>
-      <c r="K14" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1232,10 +1233,10 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F15" t="s">
         <v>35</v>
@@ -1244,13 +1245,13 @@
         <v>22</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1261,10 +1262,10 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F16" t="s">
         <v>35</v>
@@ -1273,13 +1274,13 @@
         <v>11</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J16" s="11" t="s">
         <v>12</v>
       </c>
       <c r="K16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1290,13 +1291,13 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="12" t="s">
-        <v>92</v>
-      </c>
       <c r="E17" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F17" t="s">
         <v>35</v>
@@ -1305,13 +1306,13 @@
         <v>19</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J17" s="11" t="s">
         <v>14</v>
       </c>
       <c r="K17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1319,10 +1320,10 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F18" t="s">
         <v>35</v>
@@ -1331,13 +1332,13 @@
         <v>19</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J18" s="11" t="s">
         <v>14</v>
       </c>
       <c r="K18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1348,10 +1349,10 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F19" t="s">
         <v>35</v>
@@ -1360,13 +1361,13 @@
         <v>13</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1377,7 +1378,7 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F20" t="s">
         <v>35</v>
@@ -1386,13 +1387,13 @@
         <v>15</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J20" s="11" t="s">
         <v>16</v>
       </c>
       <c r="K20" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1403,10 +1404,10 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F21" t="s">
         <v>35</v>
@@ -1421,7 +1422,7 @@
         <v>18</v>
       </c>
       <c r="K21" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1429,10 +1430,10 @@
         <v>17</v>
       </c>
       <c r="C22" t="s">
+        <v>104</v>
+      </c>
+      <c r="E22" s="11" t="s">
         <v>106</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>108</v>
       </c>
       <c r="F22" t="s">
         <v>35</v>
@@ -1447,7 +1448,7 @@
         <v>21</v>
       </c>
       <c r="K22" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1455,10 +1456,10 @@
         <v>18</v>
       </c>
       <c r="C23" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F23" t="s">
         <v>35</v>
@@ -1467,13 +1468,13 @@
         <v>23</v>
       </c>
       <c r="I23" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="J23" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="K23" t="s">
         <v>100</v>
-      </c>
-      <c r="J23" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="K23" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1481,28 +1482,28 @@
         <v>19</v>
       </c>
       <c r="C24" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F24" t="s">
         <v>35</v>
       </c>
       <c r="G24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I24" s="13">
         <v>1206</v>
       </c>
       <c r="J24" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K24" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1510,26 +1511,26 @@
         <v>20</v>
       </c>
       <c r="C25" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F25" t="s">
         <v>35</v>
       </c>
       <c r="G25" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I25" s="13">
         <v>1206</v>
       </c>
       <c r="J25" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K25" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1540,25 +1541,25 @@
         <v>733910060</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E26" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G26" t="s">
+        <v>116</v>
+      </c>
+      <c r="I26" t="s">
         <v>117</v>
       </c>
-      <c r="F26" t="s">
-        <v>35</v>
-      </c>
-      <c r="G26" t="s">
+      <c r="J26" t="s">
         <v>118</v>
       </c>
-      <c r="I26" t="s">
+      <c r="K26" t="s">
         <v>119</v>
-      </c>
-      <c r="J26" t="s">
-        <v>120</v>
-      </c>
-      <c r="K26" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -1566,25 +1567,25 @@
         <v>22</v>
       </c>
       <c r="C27" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F27" t="s">
         <v>35</v>
       </c>
       <c r="G27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I27" s="13">
         <v>1206</v>
       </c>
       <c r="J27" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -1592,25 +1593,25 @@
         <v>23</v>
       </c>
       <c r="C28" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F28" t="s">
         <v>35</v>
       </c>
       <c r="G28" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I28">
         <v>1206</v>
       </c>
       <c r="J28" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding annotations to BOM
</commit_message>
<xml_diff>
--- a/PCB/BoilermakeBadge_BOM.xlsx
+++ b/PCB/BoilermakeBadge_BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="136">
   <si>
     <t>Microcontroller</t>
   </si>
@@ -421,15 +421,6 @@
     <t>RC1206JR-0722KL</t>
   </si>
   <si>
-    <t>Customer Name:</t>
-  </si>
-  <si>
-    <t>Thomas Kilbride</t>
-  </si>
-  <si>
-    <t>Project:</t>
-  </si>
-  <si>
     <t>BoilerMakeBoard_I</t>
   </si>
   <si>
@@ -437,6 +428,21 @@
   </si>
   <si>
     <t>Battery</t>
+  </si>
+  <si>
+    <t>Assembly Part Number/Revision:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer / Company Name: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOM: </t>
+  </si>
+  <si>
+    <t>Prototype for production</t>
+  </si>
+  <si>
+    <t>Thomas Kilbride / Purdue University BoilerMake Hackathon</t>
   </si>
 </sst>
 </file>
@@ -455,14 +461,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -506,6 +504,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -542,41 +546,43 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -863,12 +869,12 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="1" max="1" width="52.85546875" customWidth="1"/>
     <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.140625" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
@@ -880,58 +886,64 @@
     <col min="13" max="13" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" t="s">
         <v>128</v>
       </c>
-      <c r="B1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>130</v>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C3" s="2"/>
-      <c r="E3" s="3"/>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:11" ht="51" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="4" t="s">
         <v>34</v>
       </c>
     </row>
@@ -945,7 +957,7 @@
       <c r="C5" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>38</v>
       </c>
       <c r="F5" t="s">
@@ -954,10 +966,10 @@
       <c r="G5" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="J5" s="10" t="s">
         <v>0</v>
       </c>
       <c r="K5" t="s">
@@ -974,8 +986,8 @@
       <c r="C6" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>132</v>
+      <c r="E6" s="10" t="s">
+        <v>129</v>
       </c>
       <c r="F6" t="s">
         <v>35</v>
@@ -983,10 +995,10 @@
       <c r="G6" t="s">
         <v>2</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="J6" s="10" t="s">
         <v>40</v>
       </c>
       <c r="K6" t="s">
@@ -1003,7 +1015,7 @@
       <c r="C7" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="10" t="s">
         <v>44</v>
       </c>
       <c r="F7" t="s">
@@ -1012,10 +1024,10 @@
       <c r="G7" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="J7" s="10" t="s">
         <v>43</v>
       </c>
       <c r="K7" t="s">
@@ -1032,8 +1044,8 @@
       <c r="C8" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="11" t="s">
-        <v>133</v>
+      <c r="E8" s="10" t="s">
+        <v>130</v>
       </c>
       <c r="F8" t="s">
         <v>35</v>
@@ -1041,10 +1053,10 @@
       <c r="G8" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="J8" s="10" t="s">
         <v>46</v>
       </c>
       <c r="K8" t="s">
@@ -1061,7 +1073,7 @@
       <c r="C9" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="10" t="s">
         <v>51</v>
       </c>
       <c r="F9" t="s">
@@ -1070,7 +1082,7 @@
       <c r="G9" t="s">
         <v>4</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="12" t="s">
         <v>54</v>
       </c>
       <c r="J9" t="s">
@@ -1090,7 +1102,7 @@
       <c r="C10" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="10" t="s">
         <v>58</v>
       </c>
       <c r="F10" t="s">
@@ -1099,7 +1111,7 @@
       <c r="G10" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="12">
         <v>1206</v>
       </c>
       <c r="J10" t="s">
@@ -1119,7 +1131,7 @@
       <c r="C11" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="10" t="s">
         <v>70</v>
       </c>
       <c r="F11" t="s">
@@ -1128,7 +1140,7 @@
       <c r="G11" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="13">
+      <c r="I11" s="12">
         <v>1206</v>
       </c>
       <c r="J11" t="s">
@@ -1148,7 +1160,7 @@
       <c r="C12" t="s">
         <v>69</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="10" t="s">
         <v>71</v>
       </c>
       <c r="F12" t="s">
@@ -1157,10 +1169,10 @@
       <c r="G12" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="I12" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="J12" s="11" t="s">
+      <c r="J12" s="10" t="s">
         <v>66</v>
       </c>
       <c r="K12" t="s">
@@ -1177,7 +1189,7 @@
       <c r="C13" t="s">
         <v>68</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="10" t="s">
         <v>82</v>
       </c>
       <c r="F13" t="s">
@@ -1186,10 +1198,10 @@
       <c r="G13" t="s">
         <v>8</v>
       </c>
-      <c r="I13" s="13">
+      <c r="I13" s="12">
         <v>1206</v>
       </c>
-      <c r="J13" s="11" t="s">
+      <c r="J13" s="10" t="s">
         <v>9</v>
       </c>
       <c r="K13" t="s">
@@ -1206,7 +1218,7 @@
       <c r="C14" t="s">
         <v>77</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="10" t="s">
         <v>76</v>
       </c>
       <c r="F14" t="s">
@@ -1215,10 +1227,10 @@
       <c r="G14" t="s">
         <v>72</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="I14" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="J14" s="11" t="s">
+      <c r="J14" s="10" t="s">
         <v>73</v>
       </c>
       <c r="K14" t="s">
@@ -1235,7 +1247,7 @@
       <c r="C15" t="s">
         <v>80</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="10" t="s">
         <v>81</v>
       </c>
       <c r="F15" t="s">
@@ -1244,7 +1256,7 @@
       <c r="G15" t="s">
         <v>22</v>
       </c>
-      <c r="I15" s="13" t="s">
+      <c r="I15" s="12" t="s">
         <v>79</v>
       </c>
       <c r="J15" t="s">
@@ -1264,7 +1276,7 @@
       <c r="C16" t="s">
         <v>86</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="10" t="s">
         <v>85</v>
       </c>
       <c r="F16" t="s">
@@ -1273,10 +1285,10 @@
       <c r="G16" t="s">
         <v>11</v>
       </c>
-      <c r="I16" s="13" t="s">
+      <c r="I16" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="J16" s="11" t="s">
+      <c r="J16" s="10" t="s">
         <v>12</v>
       </c>
       <c r="K16" t="s">
@@ -1293,22 +1305,22 @@
       <c r="C17" t="s">
         <v>88</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="10" t="s">
         <v>89</v>
       </c>
       <c r="F17" t="s">
         <v>35</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I17" s="13" t="s">
+      <c r="I17" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="J17" s="11" t="s">
+      <c r="J17" s="10" t="s">
         <v>14</v>
       </c>
       <c r="K17" t="s">
@@ -1322,19 +1334,19 @@
       <c r="C18" t="s">
         <v>88</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="10" t="s">
         <v>91</v>
       </c>
       <c r="F18" t="s">
         <v>35</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I18" s="13" t="s">
+      <c r="I18" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="J18" s="11" t="s">
+      <c r="J18" s="10" t="s">
         <v>14</v>
       </c>
       <c r="K18" t="s">
@@ -1351,7 +1363,7 @@
       <c r="C19" t="s">
         <v>97</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="10" t="s">
         <v>96</v>
       </c>
       <c r="F19" t="s">
@@ -1360,10 +1372,10 @@
       <c r="G19" t="s">
         <v>13</v>
       </c>
-      <c r="I19" s="13" t="s">
+      <c r="I19" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="J19" s="11" t="s">
+      <c r="J19" s="10" t="s">
         <v>93</v>
       </c>
       <c r="K19" t="s">
@@ -1386,10 +1398,10 @@
       <c r="G20" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="13" t="s">
+      <c r="I20" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="J20" s="11" t="s">
+      <c r="J20" s="10" t="s">
         <v>16</v>
       </c>
       <c r="K20" t="s">
@@ -1406,7 +1418,7 @@
       <c r="C21" t="s">
         <v>101</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="10" t="s">
         <v>102</v>
       </c>
       <c r="F21" t="s">
@@ -1415,10 +1427,10 @@
       <c r="G21" t="s">
         <v>17</v>
       </c>
-      <c r="I21" s="13">
+      <c r="I21" s="12">
         <v>1206</v>
       </c>
-      <c r="J21" s="11" t="s">
+      <c r="J21" s="10" t="s">
         <v>18</v>
       </c>
       <c r="K21" t="s">
@@ -1432,7 +1444,7 @@
       <c r="C22" t="s">
         <v>104</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="E22" s="10" t="s">
         <v>106</v>
       </c>
       <c r="F22" t="s">
@@ -1441,10 +1453,10 @@
       <c r="G22" t="s">
         <v>20</v>
       </c>
-      <c r="I22" s="13">
+      <c r="I22" s="12">
         <v>1206</v>
       </c>
-      <c r="J22" s="11" t="s">
+      <c r="J22" s="10" t="s">
         <v>21</v>
       </c>
       <c r="K22" t="s">
@@ -1458,7 +1470,7 @@
       <c r="C23" t="s">
         <v>107</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="E23" s="10" t="s">
         <v>108</v>
       </c>
       <c r="F23" t="s">
@@ -1467,10 +1479,10 @@
       <c r="G23" t="s">
         <v>23</v>
       </c>
-      <c r="I23" s="13" t="s">
+      <c r="I23" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="J23" s="11" t="s">
+      <c r="J23" s="10" t="s">
         <v>112</v>
       </c>
       <c r="K23" t="s">
@@ -1484,10 +1496,10 @@
       <c r="C24" t="s">
         <v>110</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="10" t="s">
         <v>113</v>
       </c>
       <c r="F24" t="s">
@@ -1496,7 +1508,7 @@
       <c r="G24" t="s">
         <v>109</v>
       </c>
-      <c r="I24" s="13">
+      <c r="I24" s="12">
         <v>1206</v>
       </c>
       <c r="J24" t="s">
@@ -1513,8 +1525,8 @@
       <c r="C25" t="s">
         <v>110</v>
       </c>
-      <c r="D25" s="12"/>
-      <c r="E25" s="11" t="s">
+      <c r="D25" s="11"/>
+      <c r="E25" s="10" t="s">
         <v>114</v>
       </c>
       <c r="F25" t="s">
@@ -1523,7 +1535,7 @@
       <c r="G25" t="s">
         <v>109</v>
       </c>
-      <c r="I25" s="13">
+      <c r="I25" s="12">
         <v>1206</v>
       </c>
       <c r="J25" t="s">
@@ -1537,13 +1549,13 @@
       <c r="A26">
         <v>21</v>
       </c>
-      <c r="C26" s="14">
+      <c r="C26" s="13">
         <v>733910060</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="E26" s="10" t="s">
         <v>115</v>
       </c>
       <c r="F26" t="s">
@@ -1569,7 +1581,7 @@
       <c r="C27" t="s">
         <v>125</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="E27" s="10" t="s">
         <v>121</v>
       </c>
       <c r="F27" t="s">
@@ -1578,7 +1590,7 @@
       <c r="G27" t="s">
         <v>120</v>
       </c>
-      <c r="I27" s="13">
+      <c r="I27" s="12">
         <v>1206</v>
       </c>
       <c r="J27" t="s">
@@ -1595,7 +1607,7 @@
       <c r="C28" t="s">
         <v>126</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="E28" s="10" t="s">
         <v>123</v>
       </c>
       <c r="F28" t="s">

</xml_diff>